<commit_message>
Class note pushed 29 June
</commit_message>
<xml_diff>
--- a/DevOps_Training.xlsx
+++ b/DevOps_Training.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/som/Desktop/DevOps Class Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E05BB665-B52A-5841-84FC-9622705AA4A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8DDD0A1-E544-D140-9EAE-9B6E54BA54E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="520" windowWidth="27180" windowHeight="17040" activeTab="7" xr2:uid="{A5538994-9363-2243-A88A-ACEBA02A2EB2}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <sheet name="Git" sheetId="6" r:id="rId6"/>
     <sheet name="Developer's Machine" sheetId="7" r:id="rId7"/>
     <sheet name="Creating Job in Jenkins" sheetId="8" r:id="rId8"/>
-    <sheet name="Crontab" sheetId="9" r:id="rId9"/>
+    <sheet name="Crontab &amp; Scripts" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="875">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1111" uniqueCount="947">
   <si>
     <t>Software Requirement</t>
   </si>
@@ -5166,12 +5166,386 @@
   <si>
     <t>Come back to Jenkins Dashboard and check if another build is created for "First_Job"</t>
   </si>
+  <si>
+    <t>Why git is required in Jenkins Master?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If there are any changes in code in github, it will be checked by Jenkins Master and not jenkins slave, </t>
+  </si>
+  <si>
+    <t>So git needs to be installed in Jenkins Master (because Jenkins Master checks if there are any changes in code in central repo (github)</t>
+  </si>
+  <si>
+    <t>Note: Empty directory will not be added to staging area and local and remote repository as well</t>
+  </si>
+  <si>
+    <t>Check with below example</t>
+  </si>
+  <si>
+    <t>login to Developer's Machine</t>
+  </si>
+  <si>
+    <t>cd /root/maven_project/myjava-web-project</t>
+  </si>
+  <si>
+    <t>#mkdir d1 d2</t>
+  </si>
+  <si>
+    <t>On branch master \nothing to commit, working directory clean</t>
+  </si>
+  <si>
+    <t>Untracked files: d2/</t>
+  </si>
+  <si>
+    <t>#touch /d2/f2 --&gt; to create a file f2 inside the directory d2</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">On branch master \ # Changes to be committed:\new file d2/f2             </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>\---&gt;consider this as next line in output</t>
+    </r>
+  </si>
+  <si>
+    <t>#git commit -m "commit for empty directory test"</t>
+  </si>
+  <si>
+    <t>1 file changed, 0 insertions(+), 0 deletions(-) -------&gt; note that file f2 is empty</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">if this doesn't work first perform "#git pull origin master" followed by </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>:q!</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (if you don't get Command Line prompt) </t>
+    </r>
+  </si>
+  <si>
+    <t>go to github and check, only directory d2 will be pushed and not d1 because d1 was empty directory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note: Even if there is no change in actual source code, but if there are any new file /directory pushed to remote central repository, </t>
+  </si>
+  <si>
+    <t>a new build will be automatically triggered (tested while checking if empty directory will be pushed to github or not)</t>
+  </si>
+  <si>
+    <t>Scripts</t>
+  </si>
+  <si>
+    <t>Scripts, also called batch file is actually a batch of commands</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">create a directory called scripts in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Developer's Machine</t>
+    </r>
+  </si>
+  <si>
+    <t>#mkdir /scripts</t>
+  </si>
+  <si>
+    <t>Create a sample file myjobs.sh inside scripts directory (.sh extention is not mandatory</t>
+  </si>
+  <si>
+    <t>#vi /scripts/myjobs.sh</t>
+  </si>
+  <si>
+    <t>free -h</t>
+  </si>
+  <si>
+    <t>df -h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">who </t>
+  </si>
+  <si>
+    <t>save and exit (ZZ or :wq!)</t>
+  </si>
+  <si>
+    <t>add list of commands you want to perform, one command each line, for example</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ls -l /scripts/myjobs.sh </t>
+  </si>
+  <si>
+    <t>-rw-r--r--. 1 root root 18 Jun 29 16:19 /scripts/myjobs.sh</t>
+  </si>
+  <si>
+    <t>chmod u+x /scripts/myjobs.sh</t>
+  </si>
+  <si>
+    <t>add execute permission to root user in myjobs.sh scripts</t>
+  </si>
+  <si>
+    <t>bash: myjobs.sh: command not found…</t>
+  </si>
+  <si>
+    <t>#myjobs.sh</t>
+  </si>
+  <si>
+    <t>/scripts/myjobs.sh</t>
+  </si>
+  <si>
+    <t>Run either with full path</t>
+  </si>
+  <si>
+    <t>cd /scripts</t>
+  </si>
+  <si>
+    <t>./myjobs.sh</t>
+  </si>
+  <si>
+    <t>or run from the directory which contains scripts</t>
+  </si>
+  <si>
+    <t>you should see output for above 3 commands put in myjobs.sh</t>
+  </si>
+  <si>
+    <t>Creating a script on a Deveoper's Machine to add, to commit and to push local changes 
+to remote (central) repository i.e. github</t>
+  </si>
+  <si>
+    <t>vi /scripts/gitupdate.sh</t>
+  </si>
+  <si>
+    <t>Extra Read: Scripts</t>
+  </si>
+  <si>
+    <t>git add -A</t>
+  </si>
+  <si>
+    <t>git commit -m "Latest Commit"</t>
+  </si>
+  <si>
+    <t>git pull origin master</t>
+  </si>
+  <si>
+    <t>git push origin master</t>
+  </si>
+  <si>
+    <t>###you can put timestamp in place of "Latest commit" to make it more professional, but we are keeping things simple</t>
+  </si>
+  <si>
+    <t>###sometimes git push origin master does not work without performing git pull origin master, when peer makes changes in code (?)</t>
+  </si>
+  <si>
+    <t>-rw-r--r--. 1 root root 324 Jun 29 16:44 /scripts/gitupdate.sh</t>
+  </si>
+  <si>
+    <t>add execute permission to root user in gitupdate.sh scripts</t>
+  </si>
+  <si>
+    <r>
+      <t>-rw</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">r--r--. 1 root root 18 Jun 29 16:19 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>/scripts/myjobs.sh</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>-rw</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">r--r--. 1 root root 324 Jun 29 16:44 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>/scripts/gitupdate.sh</t>
+    </r>
+  </si>
+  <si>
+    <t>Note Scripts will appear in green color</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Now, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">1. either run it manually </t>
+    </r>
+  </si>
+  <si>
+    <t>Or 2. Put is in Crontab</t>
+  </si>
+  <si>
+    <t>#/scripts/gitupdate.sh</t>
+  </si>
+  <si>
+    <t>#ls -l /scripts/gitupdate.sh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#ls -l /scripts/gitupdate.sh </t>
+  </si>
+  <si>
+    <t>#chmod u+x /scripts/gitupdate.sh</t>
+  </si>
+  <si>
+    <t>* * * * * /scripts/gitupdate.sh</t>
+  </si>
+  <si>
+    <t>###above scripts is made to run every minute just for lab purpose</t>
+  </si>
+  <si>
+    <t>Add below lines</t>
+  </si>
+  <si>
+    <t>Now make some change in source code (in Developer's Machine), and watch Jenkins Dashboard</t>
+  </si>
+  <si>
+    <t>add "Second edit" after the word "Hello World!"</t>
+  </si>
+  <si>
+    <t>###add below commands on file gitupdate.sh</t>
+  </si>
+  <si>
+    <t>###above line is very important as git commands won't work if not run from local repository (i.e. directory containing .git file)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">come to Jenkins Dashboard, and wait around two minutes </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>First min</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for cron job to start ---&gt; which will push changes in codes to github by git add, git commit and git push as defined in scripts</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Second minute</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to trigger auto build ---&gt; after Jenkins Master notices changes in code in github, it will trigger next build after a minute</t>
+    </r>
+  </si>
+  <si>
+    <t>Next: git different command (go to Git Tab)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="42">
+  <fonts count="43">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -5470,6 +5844,15 @@
       <color rgb="FF002060"/>
       <name val="Calibri (Body)"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF92D050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -5683,7 +6066,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -5817,6 +6200,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -5882,6 +6274,12 @@
     <xf numFmtId="0" fontId="37" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5921,7 +6319,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>671831</xdr:colOff>
+      <xdr:colOff>671830</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
@@ -5965,7 +6363,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>225410</xdr:colOff>
+      <xdr:colOff>225409</xdr:colOff>
       <xdr:row>67</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
@@ -6331,20 +6729,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="26">
-      <c r="B1" s="92" t="s">
+      <c r="B1" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="92"/>
+      <c r="C1" s="95"/>
     </row>
     <row r="2" spans="1:6" ht="20" thickBot="1">
-      <c r="B2" s="91" t="s">
+      <c r="B2" s="94" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="91"/>
-      <c r="E2" s="91" t="s">
+      <c r="C2" s="94"/>
+      <c r="E2" s="94" t="s">
         <v>92</v>
       </c>
-      <c r="F2" s="91"/>
+      <c r="F2" s="94"/>
     </row>
     <row r="3" spans="1:6">
       <c r="B3" t="s">
@@ -6392,10 +6790,10 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="19">
-      <c r="B6" s="90" t="s">
+      <c r="B6" s="93" t="s">
         <v>82</v>
       </c>
-      <c r="C6" s="90"/>
+      <c r="C6" s="93"/>
       <c r="D6" s="22">
         <v>4</v>
       </c>
@@ -6633,10 +7031,10 @@
     </row>
     <row r="28" spans="1:6" ht="20" thickBot="1">
       <c r="A28" s="1"/>
-      <c r="B28" s="90" t="s">
+      <c r="B28" s="93" t="s">
         <v>90</v>
       </c>
-      <c r="C28" s="90"/>
+      <c r="C28" s="93"/>
     </row>
     <row r="29" spans="1:6" ht="20" thickBot="1">
       <c r="A29" s="1"/>
@@ -6821,7 +7219,7 @@
     </row>
     <row r="50" spans="3:6">
       <c r="C50" s="3"/>
-      <c r="F50" s="88" t="s">
+      <c r="F50" s="91" t="s">
         <v>449</v>
       </c>
     </row>
@@ -6829,37 +7227,37 @@
       <c r="C51" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="F51" s="89"/>
+      <c r="F51" s="92"/>
     </row>
     <row r="52" spans="3:6">
       <c r="C52" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F52" s="89"/>
+      <c r="F52" s="92"/>
     </row>
     <row r="53" spans="3:6">
       <c r="C53" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F53" s="89"/>
+      <c r="F53" s="92"/>
     </row>
     <row r="54" spans="3:6">
       <c r="C54" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F54" s="89"/>
+      <c r="F54" s="92"/>
     </row>
     <row r="55" spans="3:6">
       <c r="C55" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="F55" s="89"/>
+      <c r="F55" s="92"/>
     </row>
     <row r="56" spans="3:6">
       <c r="C56" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F56" s="89"/>
+      <c r="F56" s="92"/>
     </row>
     <row r="57" spans="3:6">
       <c r="C57" s="3"/>
@@ -7311,7 +7709,7 @@
       <c r="B3" t="s">
         <v>127</v>
       </c>
-      <c r="E3" s="88" t="s">
+      <c r="E3" s="91" t="s">
         <v>202</v>
       </c>
     </row>
@@ -7319,13 +7717,13 @@
       <c r="B4" t="s">
         <v>126</v>
       </c>
-      <c r="E4" s="89"/>
+      <c r="E4" s="92"/>
     </row>
     <row r="5" spans="1:5">
       <c r="B5" t="s">
         <v>128</v>
       </c>
-      <c r="E5" s="89"/>
+      <c r="E5" s="92"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6">
@@ -7500,7 +7898,7 @@
       </c>
     </row>
     <row r="30" spans="2:5">
-      <c r="B30" s="88" t="s">
+      <c r="B30" s="91" t="s">
         <v>179</v>
       </c>
       <c r="E30" t="s">
@@ -7508,13 +7906,13 @@
       </c>
     </row>
     <row r="31" spans="2:5">
-      <c r="B31" s="88"/>
+      <c r="B31" s="91"/>
       <c r="E31" t="s">
         <v>413</v>
       </c>
     </row>
     <row r="32" spans="2:5">
-      <c r="B32" s="88"/>
+      <c r="B32" s="91"/>
       <c r="E32" t="s">
         <v>214</v>
       </c>
@@ -7528,7 +7926,7 @@
       </c>
     </row>
     <row r="34" spans="2:5">
-      <c r="B34" s="88" t="s">
+      <c r="B34" s="91" t="s">
         <v>154</v>
       </c>
       <c r="E34" t="s">
@@ -7536,10 +7934,10 @@
       </c>
     </row>
     <row r="35" spans="2:5">
-      <c r="B35" s="88"/>
+      <c r="B35" s="91"/>
     </row>
     <row r="36" spans="2:5">
-      <c r="B36" s="88"/>
+      <c r="B36" s="91"/>
       <c r="D36" s="6">
         <v>10</v>
       </c>
@@ -7662,7 +8060,7 @@
       </c>
     </row>
     <row r="53" spans="1:5">
-      <c r="E53" s="88" t="s">
+      <c r="E53" s="91" t="s">
         <v>227</v>
       </c>
     </row>
@@ -7670,7 +8068,7 @@
       <c r="B54" t="s">
         <v>161</v>
       </c>
-      <c r="E54" s="89"/>
+      <c r="E54" s="92"/>
     </row>
     <row r="55" spans="1:5">
       <c r="B55" t="s">
@@ -7681,7 +8079,7 @@
       </c>
     </row>
     <row r="56" spans="1:5">
-      <c r="B56" s="88" t="s">
+      <c r="B56" s="91" t="s">
         <v>398</v>
       </c>
       <c r="E56" t="s">
@@ -7689,7 +8087,7 @@
       </c>
     </row>
     <row r="57" spans="1:5">
-      <c r="B57" s="89"/>
+      <c r="B57" s="92"/>
       <c r="E57" t="s">
         <v>418</v>
       </c>
@@ -7897,7 +8295,7 @@
       </c>
     </row>
     <row r="85" spans="1:5">
-      <c r="B85" s="88" t="s">
+      <c r="B85" s="91" t="s">
         <v>176</v>
       </c>
       <c r="E85" t="s">
@@ -7905,7 +8303,7 @@
       </c>
     </row>
     <row r="86" spans="1:5">
-      <c r="B86" s="89"/>
+      <c r="B86" s="92"/>
       <c r="E86" t="s">
         <v>138</v>
       </c>
@@ -7922,7 +8320,7 @@
       <c r="B88" t="s">
         <v>180</v>
       </c>
-      <c r="E88" s="88" t="s">
+      <c r="E88" s="91" t="s">
         <v>435</v>
       </c>
     </row>
@@ -7930,13 +8328,13 @@
       <c r="B89" t="s">
         <v>181</v>
       </c>
-      <c r="E89" s="89"/>
+      <c r="E89" s="92"/>
     </row>
     <row r="90" spans="1:5">
       <c r="B90" t="s">
         <v>182</v>
       </c>
-      <c r="E90" s="89"/>
+      <c r="E90" s="92"/>
     </row>
     <row r="91" spans="1:5">
       <c r="B91" s="29" t="s">
@@ -7958,7 +8356,7 @@
       <c r="B93" t="s">
         <v>185</v>
       </c>
-      <c r="E93" s="88" t="s">
+      <c r="E93" s="91" t="s">
         <v>438</v>
       </c>
     </row>
@@ -7966,22 +8364,22 @@
       <c r="B94" s="27" t="s">
         <v>191</v>
       </c>
-      <c r="E94" s="88"/>
+      <c r="E94" s="91"/>
     </row>
     <row r="95" spans="1:5">
       <c r="B95" t="s">
         <v>186</v>
       </c>
-      <c r="E95" s="88"/>
+      <c r="E95" s="91"/>
     </row>
     <row r="96" spans="1:5">
-      <c r="E96" s="88"/>
+      <c r="E96" s="91"/>
     </row>
     <row r="97" spans="1:5">
       <c r="B97" s="27" t="s">
         <v>187</v>
       </c>
-      <c r="E97" s="88"/>
+      <c r="E97" s="91"/>
     </row>
     <row r="98" spans="1:5">
       <c r="B98" t="s">
@@ -8075,7 +8473,7 @@
       <c r="B109" s="27" t="s">
         <v>193</v>
       </c>
-      <c r="E109" s="93" t="s">
+      <c r="E109" s="96" t="s">
         <v>245</v>
       </c>
     </row>
@@ -8083,13 +8481,13 @@
       <c r="B110" s="27" t="s">
         <v>194</v>
       </c>
-      <c r="E110" s="94"/>
+      <c r="E110" s="97"/>
     </row>
     <row r="111" spans="1:5">
       <c r="B111" s="27" t="s">
         <v>195</v>
       </c>
-      <c r="E111" s="94"/>
+      <c r="E111" s="97"/>
     </row>
     <row r="112" spans="1:5">
       <c r="B112" s="31" t="s">
@@ -8257,7 +8655,7 @@
       <c r="B11" t="s">
         <v>251</v>
       </c>
-      <c r="D11" s="88" t="s">
+      <c r="D11" s="91" t="s">
         <v>483</v>
       </c>
     </row>
@@ -8265,13 +8663,13 @@
       <c r="B12" t="s">
         <v>454</v>
       </c>
-      <c r="D12" s="89"/>
+      <c r="D12" s="92"/>
     </row>
     <row r="13" spans="1:4">
       <c r="B13" s="2" t="s">
         <v>457</v>
       </c>
-      <c r="D13" s="89"/>
+      <c r="D13" s="92"/>
     </row>
     <row r="14" spans="1:4" ht="17" thickBot="1">
       <c r="B14" s="4" t="s">
@@ -8433,7 +8831,7 @@
       </c>
     </row>
     <row r="36" spans="2:4">
-      <c r="B36" s="88" t="s">
+      <c r="B36" s="91" t="s">
         <v>264</v>
       </c>
       <c r="D36" t="s">
@@ -8441,7 +8839,7 @@
       </c>
     </row>
     <row r="37" spans="2:4">
-      <c r="B37" s="89"/>
+      <c r="B37" s="92"/>
       <c r="D37" t="s">
         <v>307</v>
       </c>
@@ -9026,15 +9424,15 @@
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="B19" s="96" t="s">
+      <c r="B19" s="99" t="s">
         <v>530</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="B20" s="97"/>
+      <c r="B20" s="100"/>
     </row>
     <row r="21" spans="1:2" ht="17" thickBot="1">
-      <c r="B21" s="98"/>
+      <c r="B21" s="101"/>
     </row>
     <row r="22" spans="1:2">
       <c r="B22" t="s">
@@ -9118,18 +9516,18 @@
       </c>
     </row>
     <row r="42" spans="1:2">
-      <c r="B42" s="88" t="s">
+      <c r="B42" s="91" t="s">
         <v>545</v>
       </c>
     </row>
     <row r="43" spans="1:2">
-      <c r="B43" s="89"/>
+      <c r="B43" s="92"/>
     </row>
     <row r="44" spans="1:2">
-      <c r="B44" s="89"/>
+      <c r="B44" s="92"/>
     </row>
     <row r="45" spans="1:2">
-      <c r="B45" s="89"/>
+      <c r="B45" s="92"/>
     </row>
     <row r="46" spans="1:2">
       <c r="B46" s="6" t="s">
@@ -9157,12 +9555,12 @@
       </c>
     </row>
     <row r="51" spans="1:2">
-      <c r="B51" s="88" t="s">
+      <c r="B51" s="91" t="s">
         <v>552</v>
       </c>
     </row>
     <row r="52" spans="1:2">
-      <c r="B52" s="89"/>
+      <c r="B52" s="92"/>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="36" t="s">
@@ -9189,16 +9587,16 @@
       </c>
     </row>
     <row r="57" spans="1:2">
-      <c r="A57" s="95" t="s">
+      <c r="A57" s="98" t="s">
         <v>556</v>
       </c>
-      <c r="B57" s="88" t="s">
+      <c r="B57" s="91" t="s">
         <v>553</v>
       </c>
     </row>
     <row r="58" spans="1:2">
-      <c r="A58" s="95"/>
-      <c r="B58" s="89"/>
+      <c r="A58" s="98"/>
+      <c r="B58" s="92"/>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="62" t="s">
@@ -9209,20 +9607,20 @@
       </c>
     </row>
     <row r="60" spans="1:2">
-      <c r="B60" s="88" t="s">
+      <c r="B60" s="91" t="s">
         <v>558</v>
       </c>
     </row>
     <row r="61" spans="1:2">
-      <c r="B61" s="89"/>
+      <c r="B61" s="92"/>
     </row>
     <row r="62" spans="1:2">
-      <c r="B62" s="88" t="s">
+      <c r="B62" s="91" t="s">
         <v>559</v>
       </c>
     </row>
     <row r="63" spans="1:2">
-      <c r="B63" s="89"/>
+      <c r="B63" s="92"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -9317,15 +9715,15 @@
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="B16" s="88" t="s">
+      <c r="B16" s="91" t="s">
         <v>561</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="B17" s="89"/>
+      <c r="B17" s="92"/>
     </row>
     <row r="18" spans="1:2">
-      <c r="B18" s="89"/>
+      <c r="B18" s="92"/>
     </row>
     <row r="20" spans="1:2">
       <c r="B20" t="s">
@@ -9542,12 +9940,12 @@
       </c>
     </row>
     <row r="66" spans="2:2">
-      <c r="B66" s="99" t="s">
+      <c r="B66" s="102" t="s">
         <v>573</v>
       </c>
     </row>
     <row r="67" spans="2:2">
-      <c r="B67" s="100"/>
+      <c r="B67" s="103"/>
     </row>
     <row r="68" spans="2:2">
       <c r="B68" t="s">
@@ -9585,12 +9983,12 @@
       </c>
     </row>
     <row r="76" spans="2:2">
-      <c r="B76" s="89" t="s">
+      <c r="B76" s="92" t="s">
         <v>582</v>
       </c>
     </row>
     <row r="77" spans="2:2">
-      <c r="B77" s="89"/>
+      <c r="B77" s="92"/>
     </row>
     <row r="78" spans="2:2">
       <c r="B78" t="s">
@@ -9658,21 +10056,21 @@
       </c>
     </row>
     <row r="92" spans="2:2" ht="16" customHeight="1">
-      <c r="B92" s="88" t="s">
+      <c r="B92" s="91" t="s">
         <v>587</v>
       </c>
     </row>
     <row r="93" spans="2:2">
-      <c r="B93" s="88"/>
+      <c r="B93" s="91"/>
     </row>
     <row r="94" spans="2:2">
-      <c r="B94" s="88"/>
+      <c r="B94" s="91"/>
     </row>
     <row r="95" spans="2:2">
-      <c r="B95" s="88"/>
+      <c r="B95" s="91"/>
     </row>
     <row r="96" spans="2:2">
-      <c r="B96" s="88"/>
+      <c r="B96" s="91"/>
     </row>
     <row r="98" spans="2:2">
       <c r="B98" t="s">
@@ -9768,15 +10166,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38D16ACA-B0A1-7643-8229-EFBD45805710}">
-  <dimension ref="A1:J182"/>
+  <dimension ref="A1:J210"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B191" sqref="B191"/>
+    <sheetView topLeftCell="A186" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B213" sqref="B213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="2" max="2" width="90.83203125" customWidth="1"/>
+    <col min="2" max="2" width="97.6640625" customWidth="1"/>
     <col min="10" max="10" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -9904,81 +10302,81 @@
       <c r="B25" s="1" t="s">
         <v>636</v>
       </c>
-      <c r="D25" s="101" t="s">
+      <c r="D25" s="104" t="s">
         <v>682</v>
       </c>
-      <c r="E25" s="102"/>
-      <c r="F25" s="102"/>
-      <c r="G25" s="102"/>
-      <c r="H25" s="102"/>
-      <c r="I25" s="102"/>
-      <c r="J25" s="103"/>
+      <c r="E25" s="105"/>
+      <c r="F25" s="105"/>
+      <c r="G25" s="105"/>
+      <c r="H25" s="105"/>
+      <c r="I25" s="105"/>
+      <c r="J25" s="106"/>
     </row>
     <row r="26" spans="1:10" ht="19">
       <c r="B26" t="s">
         <v>637</v>
       </c>
-      <c r="D26" s="104" t="s">
+      <c r="D26" s="107" t="s">
         <v>683</v>
       </c>
-      <c r="E26" s="105"/>
-      <c r="F26" s="105"/>
-      <c r="G26" s="105"/>
-      <c r="H26" s="105"/>
-      <c r="I26" s="105"/>
-      <c r="J26" s="106"/>
+      <c r="E26" s="108"/>
+      <c r="F26" s="108"/>
+      <c r="G26" s="108"/>
+      <c r="H26" s="108"/>
+      <c r="I26" s="108"/>
+      <c r="J26" s="109"/>
     </row>
     <row r="27" spans="1:10" ht="19">
       <c r="B27" s="65" t="s">
         <v>641</v>
       </c>
-      <c r="D27" s="104" t="s">
+      <c r="D27" s="107" t="s">
         <v>681</v>
       </c>
-      <c r="E27" s="105"/>
-      <c r="F27" s="105"/>
-      <c r="G27" s="105"/>
-      <c r="H27" s="105"/>
-      <c r="I27" s="105"/>
-      <c r="J27" s="106"/>
+      <c r="E27" s="108"/>
+      <c r="F27" s="108"/>
+      <c r="G27" s="108"/>
+      <c r="H27" s="108"/>
+      <c r="I27" s="108"/>
+      <c r="J27" s="109"/>
     </row>
     <row r="28" spans="1:10" ht="20" thickBot="1">
       <c r="B28" t="s">
         <v>638</v>
       </c>
-      <c r="D28" s="107" t="s">
+      <c r="D28" s="110" t="s">
         <v>684</v>
       </c>
-      <c r="E28" s="108"/>
-      <c r="F28" s="108"/>
-      <c r="G28" s="108"/>
-      <c r="H28" s="108"/>
-      <c r="I28" s="108"/>
-      <c r="J28" s="109"/>
+      <c r="E28" s="111"/>
+      <c r="F28" s="111"/>
+      <c r="G28" s="111"/>
+      <c r="H28" s="111"/>
+      <c r="I28" s="111"/>
+      <c r="J28" s="112"/>
     </row>
     <row r="29" spans="1:10">
       <c r="B29" s="65" t="s">
         <v>640</v>
       </c>
-      <c r="D29" s="89"/>
-      <c r="E29" s="89"/>
-      <c r="F29" s="89"/>
-      <c r="G29" s="89"/>
-      <c r="H29" s="89"/>
-      <c r="I29" s="89"/>
-      <c r="J29" s="89"/>
+      <c r="D29" s="92"/>
+      <c r="E29" s="92"/>
+      <c r="F29" s="92"/>
+      <c r="G29" s="92"/>
+      <c r="H29" s="92"/>
+      <c r="I29" s="92"/>
+      <c r="J29" s="92"/>
     </row>
     <row r="30" spans="1:10">
       <c r="B30" t="s">
         <v>639</v>
       </c>
-      <c r="D30" s="89"/>
-      <c r="E30" s="89"/>
-      <c r="F30" s="89"/>
-      <c r="G30" s="89"/>
-      <c r="H30" s="89"/>
-      <c r="I30" s="89"/>
-      <c r="J30" s="89"/>
+      <c r="D30" s="92"/>
+      <c r="E30" s="92"/>
+      <c r="F30" s="92"/>
+      <c r="G30" s="92"/>
+      <c r="H30" s="92"/>
+      <c r="I30" s="92"/>
+      <c r="J30" s="92"/>
     </row>
     <row r="31" spans="1:10">
       <c r="B31" s="66" t="s">
@@ -10626,6 +11024,111 @@
     <row r="182" spans="2:2">
       <c r="B182" t="s">
         <v>772</v>
+      </c>
+    </row>
+    <row r="184" spans="2:2" ht="19">
+      <c r="B184" s="79" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="185" spans="2:2">
+      <c r="B185" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="186" spans="2:2">
+      <c r="B186" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="187" spans="2:2">
+      <c r="B187" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="188" spans="2:2">
+      <c r="B188" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="189" spans="2:2">
+      <c r="B189" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="190" spans="2:2">
+      <c r="B190" s="52" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="192" spans="2:2">
+      <c r="B192" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="193" spans="2:2">
+      <c r="B193" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="194" spans="2:2">
+      <c r="B194" s="52" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="196" spans="2:2">
+      <c r="B196" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="197" spans="2:2">
+      <c r="B197" s="52" t="s">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="199" spans="2:2">
+      <c r="B199" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="200" spans="2:2">
+      <c r="B200" t="s">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="202" spans="2:2">
+      <c r="B202" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="203" spans="2:2">
+      <c r="B203" s="52" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="205" spans="2:2">
+      <c r="B205" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="206" spans="2:2">
+      <c r="B206" s="58" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="207" spans="2:2">
+      <c r="B207" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="208" spans="2:2">
+      <c r="B208" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="210" spans="2:2">
+      <c r="B210" s="52" t="s">
+        <v>890</v>
       </c>
     </row>
   </sheetData>
@@ -10789,15 +11292,15 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B49D506-B5A3-BE44-AA5D-D388CAC6091D}">
-  <dimension ref="B1:B80"/>
+  <dimension ref="B1:B137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B117" sqref="B117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="2" max="2" width="98.33203125" customWidth="1"/>
+    <col min="2" max="2" width="112.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:2" ht="21">
@@ -11125,7 +11628,228 @@
         <v>874</v>
       </c>
     </row>
+    <row r="82" spans="2:2" ht="19">
+      <c r="B82" s="79" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2">
+      <c r="B83" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="84" spans="2:2">
+      <c r="B84" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="86" spans="2:2">
+      <c r="B86" s="76" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="87" spans="2:2">
+      <c r="B87" s="76" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="89" spans="2:2" ht="21" customHeight="1">
+      <c r="B89" s="113" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="90" spans="2:2" ht="21" customHeight="1">
+      <c r="B90" s="114"/>
+    </row>
+    <row r="92" spans="2:2" ht="19">
+      <c r="B92" s="79" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="94" spans="2:2">
+      <c r="B94" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="95" spans="2:2">
+      <c r="B95" s="52" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="96" spans="2:2">
+      <c r="B96" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2">
+      <c r="B97" s="55" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="98" spans="2:2">
+      <c r="B98" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="99" spans="2:2">
+      <c r="B99" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="100" spans="2:2">
+      <c r="B100" s="7" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="101" spans="2:2">
+      <c r="B101" s="7" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="102" spans="2:2">
+      <c r="B102" s="7" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="103" spans="2:2">
+      <c r="B103" t="s">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="105" spans="2:2">
+      <c r="B105" s="52" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="107" spans="2:2">
+      <c r="B107" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="109" spans="2:2">
+      <c r="B109" s="86" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="110" spans="2:2">
+      <c r="B110" s="52" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="111" spans="2:2">
+      <c r="B111" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="113" spans="2:2">
+      <c r="B113" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="114" spans="2:2">
+      <c r="B114" s="86" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="115" spans="2:2">
+      <c r="B115" s="90" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="117" spans="2:2" ht="19">
+      <c r="B117" t="s">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="118" spans="2:2">
+      <c r="B118" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="120" spans="2:2">
+      <c r="B120" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="121" spans="2:2">
+      <c r="B121" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="122" spans="2:2">
+      <c r="B122" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="123" spans="2:2">
+      <c r="B123" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="124" spans="2:2">
+      <c r="B124" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="125" spans="2:2">
+      <c r="B125" s="65" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="127" spans="2:2">
+      <c r="B127" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="128" spans="2:2">
+      <c r="B128" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="129" spans="2:2">
+      <c r="B129" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="130" spans="2:2">
+      <c r="B130" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="131" spans="2:2">
+      <c r="B131" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="132" spans="2:2">
+      <c r="B132" s="65" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="133" spans="2:2">
+      <c r="B133" s="76" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="134" spans="2:2">
+      <c r="B134" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="135" spans="2:2">
+      <c r="B135" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="137" spans="2:2">
+      <c r="B137" s="76" t="s">
+        <v>946</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B89:B90"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -11133,10 +11857,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EFFC15A-91DD-B746-B11F-91C4FA60B453}">
-  <dimension ref="B1:G31"/>
+  <dimension ref="B1:I31"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView topLeftCell="C10" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -11144,46 +11868,59 @@
     <col min="2" max="2" width="24" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
     <col min="7" max="7" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="67.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="21">
+    <row r="1" spans="2:9" ht="21">
       <c r="B1" s="43" t="s">
         <v>827</v>
       </c>
-    </row>
-    <row r="2" spans="2:7">
+      <c r="I1" s="43" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="2" spans="2:9">
       <c r="B2" t="s">
         <v>828</v>
       </c>
       <c r="C2" t="s">
         <v>829</v>
       </c>
-    </row>
-    <row r="3" spans="2:7">
-      <c r="B3" s="89" t="s">
+      <c r="I2" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9">
+      <c r="B3" s="92" t="s">
         <v>830</v>
       </c>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-    </row>
-    <row r="4" spans="2:7" ht="17" thickBot="1">
+      <c r="C3" s="92"/>
+      <c r="D3" s="92"/>
+      <c r="E3" s="92"/>
+      <c r="F3" s="92"/>
+    </row>
+    <row r="4" spans="2:9" ht="17" thickBot="1">
       <c r="B4" t="s">
         <v>831</v>
       </c>
-    </row>
-    <row r="5" spans="2:7" ht="17" thickBot="1">
-      <c r="B5" s="110" t="s">
+      <c r="I4" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" ht="17" thickBot="1">
+      <c r="B5" s="115" t="s">
         <v>832</v>
       </c>
-      <c r="C5" s="111"/>
-      <c r="D5" s="111"/>
-      <c r="E5" s="111"/>
-      <c r="F5" s="111"/>
-      <c r="G5" s="112"/>
-    </row>
-    <row r="6" spans="2:7" ht="17" thickBot="1">
+      <c r="C5" s="116"/>
+      <c r="D5" s="116"/>
+      <c r="E5" s="116"/>
+      <c r="F5" s="116"/>
+      <c r="G5" s="117"/>
+      <c r="I5" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" ht="17" thickBot="1">
       <c r="B6" s="73" t="s">
         <v>833</v>
       </c>
@@ -11202,8 +11939,11 @@
       <c r="G6" s="74" t="s">
         <v>838</v>
       </c>
-    </row>
-    <row r="7" spans="2:7">
+      <c r="I6" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9">
       <c r="B7" s="84" t="s">
         <v>839</v>
       </c>
@@ -11222,8 +11962,11 @@
       <c r="G7" t="s">
         <v>844</v>
       </c>
-    </row>
-    <row r="8" spans="2:7">
+      <c r="I7" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9">
       <c r="B8" s="84" t="s">
         <v>857</v>
       </c>
@@ -11239,8 +11982,11 @@
       <c r="F8" t="s">
         <v>848</v>
       </c>
-    </row>
-    <row r="9" spans="2:7">
+      <c r="I8" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9">
       <c r="B9" s="84" t="s">
         <v>858</v>
       </c>
@@ -11256,8 +12002,11 @@
       <c r="F9" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="10" spans="2:7">
+      <c r="I9" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9">
       <c r="B10" s="84" t="s">
         <v>859</v>
       </c>
@@ -11273,8 +12022,16 @@
       <c r="F10" t="s">
         <v>850</v>
       </c>
-    </row>
-    <row r="12" spans="2:7" ht="17" thickBot="1">
+      <c r="I10" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9">
+      <c r="I11" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" ht="17" thickBot="1">
       <c r="B12" s="42" t="s">
         <v>860</v>
       </c>
@@ -11293,18 +12050,26 @@
       <c r="G12" s="42" t="s">
         <v>861</v>
       </c>
-    </row>
-    <row r="13" spans="2:7" ht="17" thickBot="1">
-      <c r="B13" s="110" t="s">
+      <c r="I12" s="65" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" ht="17" thickBot="1">
+      <c r="B13" s="115" t="s">
         <v>862</v>
       </c>
-      <c r="C13" s="111"/>
-      <c r="D13" s="111"/>
-      <c r="E13" s="111"/>
-      <c r="F13" s="111"/>
-      <c r="G13" s="112"/>
-    </row>
-    <row r="15" spans="2:7" ht="17" thickBot="1">
+      <c r="C13" s="116"/>
+      <c r="D13" s="116"/>
+      <c r="E13" s="116"/>
+      <c r="F13" s="116"/>
+      <c r="G13" s="117"/>
+    </row>
+    <row r="14" spans="2:9">
+      <c r="I14" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" ht="17" thickBot="1">
       <c r="B15" s="42" t="s">
         <v>863</v>
       </c>
@@ -11323,18 +12088,26 @@
       <c r="G15" s="42" t="s">
         <v>861</v>
       </c>
-    </row>
-    <row r="16" spans="2:7" ht="17" thickBot="1">
-      <c r="B16" s="110" t="s">
+      <c r="I15" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" ht="17" thickBot="1">
+      <c r="B16" s="115" t="s">
         <v>864</v>
       </c>
-      <c r="C16" s="111"/>
-      <c r="D16" s="111"/>
-      <c r="E16" s="111"/>
-      <c r="F16" s="111"/>
-      <c r="G16" s="112"/>
-    </row>
-    <row r="18" spans="2:7" ht="17" thickBot="1">
+      <c r="C16" s="116"/>
+      <c r="D16" s="116"/>
+      <c r="E16" s="116"/>
+      <c r="F16" s="116"/>
+      <c r="G16" s="117"/>
+    </row>
+    <row r="17" spans="2:9">
+      <c r="I17" s="52" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" ht="17" thickBot="1">
       <c r="B18" s="42" t="s">
         <v>865</v>
       </c>
@@ -11353,18 +12126,26 @@
       <c r="G18" s="42" t="s">
         <v>861</v>
       </c>
-    </row>
-    <row r="19" spans="2:7" ht="17" thickBot="1">
-      <c r="B19" s="110" t="s">
+      <c r="I18" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" ht="17" thickBot="1">
+      <c r="B19" s="115" t="s">
         <v>866</v>
       </c>
-      <c r="C19" s="111"/>
-      <c r="D19" s="111"/>
-      <c r="E19" s="111"/>
-      <c r="F19" s="111"/>
-      <c r="G19" s="112"/>
-    </row>
-    <row r="21" spans="2:7" ht="17" thickBot="1">
+      <c r="C19" s="116"/>
+      <c r="D19" s="116"/>
+      <c r="E19" s="116"/>
+      <c r="F19" s="116"/>
+      <c r="G19" s="117"/>
+    </row>
+    <row r="20" spans="2:9">
+      <c r="I20" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" ht="17" thickBot="1">
       <c r="B21" s="87" t="s">
         <v>867</v>
       </c>
@@ -11383,18 +12164,26 @@
       <c r="G21" s="42" t="s">
         <v>861</v>
       </c>
-    </row>
-    <row r="22" spans="2:7" ht="17" thickBot="1">
-      <c r="B22" s="110" t="s">
+      <c r="I21" s="89" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" ht="17" thickBot="1">
+      <c r="B22" s="115" t="s">
         <v>868</v>
       </c>
-      <c r="C22" s="111"/>
-      <c r="D22" s="111"/>
-      <c r="E22" s="111"/>
-      <c r="F22" s="111"/>
-      <c r="G22" s="112"/>
-    </row>
-    <row r="24" spans="2:7" ht="17" thickBot="1">
+      <c r="C22" s="116"/>
+      <c r="D22" s="116"/>
+      <c r="E22" s="116"/>
+      <c r="F22" s="116"/>
+      <c r="G22" s="117"/>
+    </row>
+    <row r="23" spans="2:9">
+      <c r="I23" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" ht="17" thickBot="1">
       <c r="B24" s="42" t="s">
         <v>860</v>
       </c>
@@ -11413,18 +12202,26 @@
       <c r="G24" s="42" t="s">
         <v>861</v>
       </c>
-    </row>
-    <row r="25" spans="2:7" ht="17" thickBot="1">
-      <c r="B25" s="110" t="s">
+      <c r="I24" s="52" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" ht="17" thickBot="1">
+      <c r="B25" s="115" t="s">
         <v>870</v>
       </c>
-      <c r="C25" s="111"/>
-      <c r="D25" s="111"/>
-      <c r="E25" s="111"/>
-      <c r="F25" s="111"/>
-      <c r="G25" s="112"/>
-    </row>
-    <row r="27" spans="2:7" ht="17" thickBot="1">
+      <c r="C25" s="116"/>
+      <c r="D25" s="116"/>
+      <c r="E25" s="116"/>
+      <c r="F25" s="116"/>
+      <c r="G25" s="117"/>
+    </row>
+    <row r="26" spans="2:9">
+      <c r="I26" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" ht="17" thickBot="1">
       <c r="B27" s="87" t="s">
         <v>867</v>
       </c>
@@ -11443,18 +12240,29 @@
       <c r="G27" s="42" t="s">
         <v>861</v>
       </c>
-    </row>
-    <row r="28" spans="2:7" ht="17" thickBot="1">
-      <c r="B28" s="110" t="s">
+      <c r="I27" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" ht="17" thickBot="1">
+      <c r="B28" s="115" t="s">
         <v>871</v>
       </c>
-      <c r="C28" s="111"/>
-      <c r="D28" s="111"/>
-      <c r="E28" s="111"/>
-      <c r="F28" s="111"/>
-      <c r="G28" s="112"/>
-    </row>
-    <row r="30" spans="2:7" ht="17" thickBot="1">
+      <c r="C28" s="116"/>
+      <c r="D28" s="116"/>
+      <c r="E28" s="116"/>
+      <c r="F28" s="116"/>
+      <c r="G28" s="117"/>
+      <c r="I28" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9">
+      <c r="I29" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" ht="17" thickBot="1">
       <c r="B30" s="87">
         <v>59</v>
       </c>
@@ -11473,16 +12281,22 @@
       <c r="G30" s="42" t="s">
         <v>861</v>
       </c>
-    </row>
-    <row r="31" spans="2:7" ht="17" thickBot="1">
-      <c r="B31" s="110" t="s">
+      <c r="I30" s="88" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" ht="17" thickBot="1">
+      <c r="B31" s="115" t="s">
         <v>872</v>
       </c>
-      <c r="C31" s="111"/>
-      <c r="D31" s="111"/>
-      <c r="E31" s="111"/>
-      <c r="F31" s="111"/>
-      <c r="G31" s="112"/>
+      <c r="C31" s="116"/>
+      <c r="D31" s="116"/>
+      <c r="E31" s="116"/>
+      <c r="F31" s="116"/>
+      <c r="G31" s="117"/>
+      <c r="I31" s="52" t="s">
+        <v>915</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>